<commit_message>
Added Search and agenda designs
Added the search and agenda .xd files, also added a pdf version for easy viewing. Modified the url list because two were missing.
</commit_message>
<xml_diff>
--- a/documentation/excel:word:xd files/url_list.xlsx
+++ b/documentation/excel:word:xd files/url_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robbe/Desktop/school/ma/bewijzenmap/periode1.4/PROJ/MyBand-Starter/documentation/excel:word files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robbe/Desktop/school/ma/bewijzenmap/periode1.4/PROJ/MyBand-Starter/documentation/excel:word:xd files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{325372FA-1308-3B44-98EA-38B0390DF871}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC10CBB0-B03F-5A43-9F99-C55AD49B5F76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A6C97AC6-0EAB-574B-8A4C-D6B8C59546B7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{A6C97AC6-0EAB-574B-8A4C-D6B8C59546B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Where</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>The-chain.nl/story</t>
+  </si>
+  <si>
+    <t>Boots</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>The-chain.nl/story/characters/boots</t>
+  </si>
+  <si>
+    <t>The-chain.nl/story/characters/king</t>
   </si>
 </sst>
 </file>
@@ -467,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{189A9C4C-0C40-2745-B65F-941014007358}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,6 +595,22 @@
         <v>25</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>